<commit_message>
table to column macro, vlookup
add macro to pivot table.xlsm, add reference for vlookup, add formula to
combine column header and row header with the cell content. tomorrow
need to test multiple criteria vlookup because some duplicate lengths.
</commit_message>
<xml_diff>
--- a/for Hector/pivot table.xlsx
+++ b/for Hector/pivot table.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet5" sheetId="12" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="14" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId3"/>
+    <sheet name="formula" sheetId="9" r:id="rId3"/>
     <sheet name="p chart" sheetId="2" r:id="rId4"/>
     <sheet name="p table" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="15" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="12" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="14" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="117">
   <si>
     <t>Year</t>
   </si>
@@ -240,9 +241,6 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Count of Length</t>
-  </si>
-  <si>
     <t>L2</t>
   </si>
   <si>
@@ -280,6 +278,102 @@
   </si>
   <si>
     <t>treatment 4 Total</t>
+  </si>
+  <si>
+    <t>EA000001</t>
+  </si>
+  <si>
+    <t>EA000002</t>
+  </si>
+  <si>
+    <t>EA000003</t>
+  </si>
+  <si>
+    <t>EA000004</t>
+  </si>
+  <si>
+    <t>EA000005</t>
+  </si>
+  <si>
+    <t>EA000006</t>
+  </si>
+  <si>
+    <t>EA000007</t>
+  </si>
+  <si>
+    <t>EA000008</t>
+  </si>
+  <si>
+    <t>EA000009</t>
+  </si>
+  <si>
+    <t>EA000010</t>
+  </si>
+  <si>
+    <t>EA000011</t>
+  </si>
+  <si>
+    <t>EA000012</t>
+  </si>
+  <si>
+    <t>EA000013</t>
+  </si>
+  <si>
+    <t>EA000014</t>
+  </si>
+  <si>
+    <t>EA000015</t>
+  </si>
+  <si>
+    <t>EA000016</t>
+  </si>
+  <si>
+    <t>EA000017</t>
+  </si>
+  <si>
+    <t>EA000018</t>
+  </si>
+  <si>
+    <t>EA000019</t>
+  </si>
+  <si>
+    <t>EA000020</t>
+  </si>
+  <si>
+    <t>EA000021</t>
+  </si>
+  <si>
+    <t>EA000022</t>
+  </si>
+  <si>
+    <t>EA000023</t>
+  </si>
+  <si>
+    <t>EA000024</t>
+  </si>
+  <si>
+    <t>Treatment 01</t>
+  </si>
+  <si>
+    <t>Treatment 02</t>
+  </si>
+  <si>
+    <t>Treatment 03</t>
+  </si>
+  <si>
+    <t>Treatment 04</t>
+  </si>
+  <si>
+    <t>Treatment 05</t>
+  </si>
+  <si>
+    <t>Treatment 06</t>
+  </si>
+  <si>
+    <t>Treatment 07</t>
+  </si>
+  <si>
+    <t>Treatment 08</t>
   </si>
 </sst>
 </file>
@@ -361,7 +455,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[pivot table.xlsx]Sheet5!PivotTable3</c:name>
+    <c:name>[pivot table.xlsx]Sheet2!PivotTable2</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -369,181 +463,27 @@
     <c:pivotFmts>
       <c:pivotFmt>
         <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="3"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:marker>
           <c:symbol val="none"/>
         </c:marker>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="4"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="80000"/>
-              <a:lumOff val="20000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="5"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent2">
-              <a:lumMod val="80000"/>
-              <a:lumOff val="20000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:layout/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="1"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-              <c15:layout/>
-            </c:ext>
-          </c:extLst>
-        </c:dLbl>
       </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
@@ -557,28 +497,19 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$B$1:$B$4</c:f>
+              <c:f>Sheet2!$B$1:$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 1 - 100009</c:v>
+                  <c:v> L2 - treatment 1 - EA000009</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -604,12 +535,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$B$5:$B$11</c:f>
+              <c:f>Sheet2!$B$5:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>11.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -620,28 +551,19 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$D$1:$D$4</c:f>
+              <c:f>Sheet2!$D$1:$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 2 - 100010</c:v>
+                  <c:v> L2 - treatment 2 - EA000010</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -667,12 +589,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$D$5:$D$11</c:f>
+              <c:f>Sheet2!$D$5:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -683,28 +605,19 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$F$1:$F$4</c:f>
+              <c:f>Sheet2!$F$1:$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 3 - 100007</c:v>
+                  <c:v> L2 - treatment 3 - EA000007</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -730,12 +643,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$F$5:$F$11</c:f>
+              <c:f>Sheet2!$F$5:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -746,28 +659,19 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$G$1:$G$4</c:f>
+              <c:f>Sheet2!$G$1:$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 3 - 100011</c:v>
+                  <c:v> L2 - treatment 3 - EA000011</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -793,12 +697,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$G$5:$G$11</c:f>
+              <c:f>Sheet2!$G$5:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -809,28 +713,19 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$I$1:$I$4</c:f>
+              <c:f>Sheet2!$I$1:$I$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 4 - 100008</c:v>
+                  <c:v> L2 - treatment 4 - EA000008</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -856,12 +751,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$I$5:$I$11</c:f>
+              <c:f>Sheet2!$I$5:$I$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>7.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -872,28 +767,19 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$J$1:$J$4</c:f>
+              <c:f>Sheet2!$J$1:$J$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L2 - treatment 4 - 100012</c:v>
+                  <c:v> L2 - treatment 4 - EA000012</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -919,12 +805,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$J$5:$J$11</c:f>
+              <c:f>Sheet2!$J$5:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3.077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,30 +821,19 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$M$1:$M$4</c:f>
+              <c:f>Sheet2!$M$1:$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 1 - 100013</c:v>
+                  <c:v> L3 - treatment 1 - EA000013</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -984,12 +859,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$M$5:$M$11</c:f>
+              <c:f>Sheet2!$M$5:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5.77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1000,30 +875,19 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$N$1:$N$4</c:f>
+              <c:f>Sheet2!$N$1:$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 1 - 100017</c:v>
+                  <c:v> L3 - treatment 1 - EA000017</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1049,7 +913,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$N$5:$N$11</c:f>
+              <c:f>Sheet2!$N$5:$N$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1062,30 +926,19 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$P$1:$P$4</c:f>
+              <c:f>Sheet2!$P$1:$P$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 2 - 100014</c:v>
+                  <c:v> L3 - treatment 2 - EA000014</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1111,12 +964,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$P$5:$P$11</c:f>
+              <c:f>Sheet2!$P$5:$P$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,30 +980,19 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$Q$1:$Q$4</c:f>
+              <c:f>Sheet2!$Q$1:$Q$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 2 - 100018</c:v>
+                  <c:v> L3 - treatment 2 - EA000018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1176,12 +1018,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$Q$5:$Q$11</c:f>
+              <c:f>Sheet2!$Q$5:$Q$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1192,30 +1034,19 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$S$1:$S$4</c:f>
+              <c:f>Sheet2!$S$1:$S$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 3 - 100015</c:v>
+                  <c:v> L3 - treatment 3 - EA000015</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1241,7 +1072,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$S$5:$S$11</c:f>
+              <c:f>Sheet2!$S$5:$S$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1254,30 +1085,19 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$U$1:$U$4</c:f>
+              <c:f>Sheet2!$U$1:$U$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L3 - treatment 4 - 100016</c:v>
+                  <c:v> L3 - treatment 4 - EA000016</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1303,12 +1123,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$U$5:$U$11</c:f>
+              <c:f>Sheet2!$U$5:$U$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>11.807</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1319,31 +1139,19 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$X$1:$X$4</c:f>
+              <c:f>Sheet2!$X$1:$X$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 1 - 100021</c:v>
+                  <c:v> L4 - treatment 1 - EA000021</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1369,7 +1177,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$X$5:$X$11</c:f>
+              <c:f>Sheet2!$X$5:$X$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1382,104 +1190,19 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$Z$1:$Z$4</c:f>
+              <c:f>Sheet2!$Z$1:$Z$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 2 - 100022</c:v>
+                  <c:v> L4 - treatment 2 - EA000022</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="1"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1505,12 +1228,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$Z$5:$Z$11</c:f>
+              <c:f>Sheet2!$Z$5:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3.69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1521,31 +1244,19 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AB$1:$AB$4</c:f>
+              <c:f>Sheet2!$AB$1:$AB$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 3 - 100019</c:v>
+                  <c:v> L4 - treatment 3 - EA000019</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1571,12 +1282,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AB$5:$AB$11</c:f>
+              <c:f>Sheet2!$AB$5:$AB$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1587,31 +1298,19 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AC$1:$AC$4</c:f>
+              <c:f>Sheet2!$AC$1:$AC$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 3 - 100023</c:v>
+                  <c:v> L4 - treatment 3 - EA000023</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1637,7 +1336,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AC$5:$AC$11</c:f>
+              <c:f>Sheet2!$AC$5:$AC$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1650,31 +1349,19 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AE$1:$AE$4</c:f>
+              <c:f>Sheet2!$AE$1:$AE$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 4 - 100020</c:v>
+                  <c:v> L4 - treatment 4 - EA000020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1700,12 +1387,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AE$5:$AE$11</c:f>
+              <c:f>Sheet2!$AE$5:$AE$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>14.611000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1716,31 +1403,19 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AF$1:$AF$4</c:f>
+              <c:f>Sheet2!$AF$1:$AF$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> L4 - treatment 4 - 100024</c:v>
+                  <c:v> L4 - treatment 4 - EA000024</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="80000"/>
-                <a:lumOff val="20000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1766,12 +1441,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AF$5:$AF$11</c:f>
+              <c:f>Sheet2!$AF$5:$AF$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1782,30 +1457,19 @@
           <c:order val="18"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AI$1:$AI$4</c:f>
+              <c:f>Sheet2!$AI$1:$AI$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 1 - 100001</c:v>
+                  <c:v>L1 - treatment 1 - EA000001</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1831,12 +1495,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AI$5:$AI$11</c:f>
+              <c:f>Sheet2!$AI$5:$AI$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>10.039999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,30 +1511,19 @@
           <c:order val="19"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AJ$1:$AJ$4</c:f>
+              <c:f>Sheet2!$AJ$1:$AJ$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 1 - 100005</c:v>
+                  <c:v>L1 - treatment 1 - EA000005</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1896,7 +1549,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AJ$5:$AJ$11</c:f>
+              <c:f>Sheet2!$AJ$5:$AJ$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1909,30 +1562,19 @@
           <c:order val="20"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AL$1:$AL$4</c:f>
+              <c:f>Sheet2!$AL$1:$AL$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 2 - 100002</c:v>
+                  <c:v>L1 - treatment 2 - EA000002</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -1958,7 +1600,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AL$5:$AL$11</c:f>
+              <c:f>Sheet2!$AL$5:$AL$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1971,30 +1613,19 @@
           <c:order val="21"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AM$1:$AM$4</c:f>
+              <c:f>Sheet2!$AM$1:$AM$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 2 - 100006</c:v>
+                  <c:v>L1 - treatment 2 - EA000006</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2020,7 +1651,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AM$5:$AM$11</c:f>
+              <c:f>Sheet2!$AM$5:$AM$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2033,30 +1664,19 @@
           <c:order val="22"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AO$1:$AO$4</c:f>
+              <c:f>Sheet2!$AO$1:$AO$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 3 - 100003</c:v>
+                  <c:v>L1 - treatment 3 - EA000003</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2082,12 +1702,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AO$5:$AO$11</c:f>
+              <c:f>Sheet2!$AO$5:$AO$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>6.7770000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2098,30 +1718,19 @@
           <c:order val="23"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet5!$AQ$1:$AQ$4</c:f>
+              <c:f>Sheet2!$AQ$1:$AQ$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>L1 - treatment 4 - 100004</c:v>
+                  <c:v>L1 - treatment 4 - EA000004</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="80000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet5!$A$5:$A$11</c:f>
+              <c:f>Sheet2!$A$5:$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
@@ -2147,12 +1756,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet5!$AQ$5:$AQ$11</c:f>
+              <c:f>Sheet2!$AQ$5:$AQ$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>8.5670000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,54 +1777,20 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="352636608"/>
-        <c:axId val="352637000"/>
+        <c:axId val="35081216"/>
+        <c:axId val="85252288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="352636608"/>
+        <c:axId val="35081216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="352637000"/>
+        <c:crossAx val="85252288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,130 +1798,31 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="352637000"/>
+        <c:axId val="85252288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="352636608"/>
+        <c:crossAx val="35081216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2541,17 +2017,6 @@
               <c:y val="1.8315018315017979E-3"/>
             </c:manualLayout>
           </c:layout>
-          <c:spPr/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -2575,17 +2040,6 @@
               <c:y val="1.8315018315018315E-3"/>
             </c:manualLayout>
           </c:layout>
-          <c:spPr/>
-          <c:txPr>
-            <a:bodyPr/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr/>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
           <c:showLegendKey val="0"/>
           <c:showVal val="1"/>
           <c:showCatName val="0"/>
@@ -3250,12 +2704,6 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3315,11 +2763,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="174100768"/>
-        <c:axId val="174101160"/>
+        <c:axId val="522907136"/>
+        <c:axId val="538084480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="174100768"/>
+        <c:axId val="522907136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,7 +2777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174101160"/>
+        <c:crossAx val="538084480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3337,7 +2785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174101160"/>
+        <c:axId val="538084480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -3349,7 +2797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174100768"/>
+        <c:crossAx val="522907136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3376,565 +2824,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:colOff>628650</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4035,9 +2938,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="41878.651849189817" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="41878.781163310188" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="24">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:E25" sheet="data" r:id="rId2"/>
+    <worksheetSource ref="A1:E25" sheet="data"/>
   </cacheSource>
   <cacheFields count="5">
     <cacheField name="Year" numFmtId="0">
@@ -4070,31 +2973,31 @@
       </sharedItems>
     </cacheField>
     <cacheField name="EA" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="100001" maxValue="100024" count="24">
-        <n v="100001"/>
-        <n v="100002"/>
-        <n v="100003"/>
-        <n v="100004"/>
-        <n v="100005"/>
-        <n v="100006"/>
-        <n v="100007"/>
-        <n v="100008"/>
-        <n v="100009"/>
-        <n v="100010"/>
-        <n v="100011"/>
-        <n v="100012"/>
-        <n v="100013"/>
-        <n v="100014"/>
-        <n v="100015"/>
-        <n v="100016"/>
-        <n v="100017"/>
-        <n v="100018"/>
-        <n v="100019"/>
-        <n v="100020"/>
-        <n v="100021"/>
-        <n v="100022"/>
-        <n v="100023"/>
-        <n v="100024"/>
+      <sharedItems count="24">
+        <s v="EA000001"/>
+        <s v="EA000002"/>
+        <s v="EA000003"/>
+        <s v="EA000004"/>
+        <s v="EA000005"/>
+        <s v="EA000006"/>
+        <s v="EA000007"/>
+        <s v="EA000008"/>
+        <s v="EA000009"/>
+        <s v="EA000010"/>
+        <s v="EA000011"/>
+        <s v="EA000012"/>
+        <s v="EA000013"/>
+        <s v="EA000014"/>
+        <s v="EA000015"/>
+        <s v="EA000016"/>
+        <s v="EA000017"/>
+        <s v="EA000018"/>
+        <s v="EA000019"/>
+        <s v="EA000020"/>
+        <s v="EA000021"/>
+        <s v="EA000022"/>
+        <s v="EA000023"/>
+        <s v="EA000024"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -4429,7 +3332,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:AT11" firstHeaderRow="1" firstDataRow="4" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" showAll="0">
@@ -4681,9 +3584,9 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Length" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Length" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="6">
+  <chartFormats count="4">
     <chartFormat chart="0" format="0" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -4716,45 +3619,6 @@
         <references count="1">
           <reference field="1" count="1" selected="0">
             <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="4">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="21"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="5">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="21"/>
           </reference>
         </references>
       </pivotArea>
@@ -5145,7 +4009,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5180,7 +4044,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5395,23 +4259,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.42578125" customWidth="1"/>
     <col min="12" max="12" width="8.140625" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.28515625" customWidth="1"/>
-    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="17" max="17" width="9.28515625" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -5423,17 +4287,17 @@
     <col min="26" max="26" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7" customWidth="1"/>
+    <col min="29" max="29" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="7" customWidth="1"/>
+    <col min="32" max="32" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.140625" customWidth="1"/>
     <col min="35" max="35" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7" customWidth="1"/>
+    <col min="36" max="36" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="7" customWidth="1"/>
+    <col min="39" max="39" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -5445,7 +4309,7 @@
   <sheetData>
     <row r="1" spans="1:46">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -5482,177 +4346,177 @@
     </row>
     <row r="3" spans="1:46">
       <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" t="s">
         <v>78</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>83</v>
       </c>
-      <c r="F3" t="s">
+      <c r="I3" t="s">
         <v>80</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" t="s">
         <v>81</v>
       </c>
-      <c r="K3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>78</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>82</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>79</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>83</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>80</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>84</v>
       </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y3" t="s">
         <v>81</v>
       </c>
-      <c r="V3" t="s">
-        <v>85</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>78</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
         <v>82</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AD3" t="s">
         <v>83</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AE3" t="s">
         <v>80</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AG3" t="s">
         <v>84</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AI3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK3" t="s">
         <v>81</v>
       </c>
-      <c r="AG3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI3" t="s">
+      <c r="AL3" t="s">
         <v>78</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AN3" t="s">
         <v>82</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AO3" t="s">
         <v>79</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AP3" t="s">
         <v>83</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AQ3" t="s">
         <v>80</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AR3" t="s">
         <v>84</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:46">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>100009</v>
-      </c>
-      <c r="D4">
-        <v>100010</v>
-      </c>
-      <c r="F4">
-        <v>100007</v>
-      </c>
-      <c r="G4">
-        <v>100011</v>
-      </c>
-      <c r="I4">
-        <v>100008</v>
-      </c>
-      <c r="J4">
-        <v>100012</v>
-      </c>
-      <c r="M4">
-        <v>100013</v>
-      </c>
-      <c r="N4">
-        <v>100017</v>
-      </c>
-      <c r="P4">
-        <v>100014</v>
-      </c>
-      <c r="Q4">
-        <v>100018</v>
-      </c>
-      <c r="S4">
-        <v>100015</v>
-      </c>
-      <c r="U4">
-        <v>100016</v>
-      </c>
-      <c r="X4">
-        <v>100021</v>
-      </c>
-      <c r="Z4">
-        <v>100022</v>
-      </c>
-      <c r="AB4">
-        <v>100019</v>
-      </c>
-      <c r="AC4">
-        <v>100023</v>
-      </c>
-      <c r="AE4">
-        <v>100020</v>
-      </c>
-      <c r="AF4">
-        <v>100024</v>
-      </c>
-      <c r="AI4">
-        <v>100001</v>
-      </c>
-      <c r="AJ4">
-        <v>100005</v>
-      </c>
-      <c r="AL4">
-        <v>100002</v>
-      </c>
-      <c r="AM4">
-        <v>100006</v>
-      </c>
-      <c r="AO4">
-        <v>100003</v>
-      </c>
-      <c r="AQ4">
-        <v>100004</v>
+      <c r="B4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>97</v>
+      </c>
+      <c r="N4" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>102</v>
+      </c>
+      <c r="S4" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" t="s">
+        <v>100</v>
+      </c>
+      <c r="X4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:46">
@@ -5664,24 +4528,24 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
-        <v>1</v>
+        <v>3.99</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3">
-        <v>1</v>
+        <v>3.99</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3">
-        <v>1</v>
+        <v>3.99</v>
       </c>
       <c r="M5" s="3">
-        <v>1</v>
+        <v>5.77</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3">
-        <v>1</v>
+        <v>5.77</v>
       </c>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
@@ -5691,31 +4555,31 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3">
-        <v>1</v>
+        <v>5.77</v>
       </c>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="AI5" s="3">
-        <v>1</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3">
-        <v>1</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AL5" s="3"/>
       <c r="AM5" s="3"/>
@@ -5725,10 +4589,10 @@
       <c r="AQ5" s="3"/>
       <c r="AR5" s="3"/>
       <c r="AS5" s="3">
-        <v>1</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AT5" s="3">
-        <v>4</v>
+        <v>24.099999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:46">
@@ -5743,31 +4607,31 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3">
-        <v>1</v>
+        <v>7.27</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3">
-        <v>1</v>
+        <v>7.27</v>
       </c>
       <c r="L6" s="3">
-        <v>1</v>
+        <v>7.27</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3">
-        <v>1</v>
+        <v>2.61</v>
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3">
-        <v>1</v>
+        <v>2.61</v>
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3">
-        <v>1</v>
+        <v>2.61</v>
       </c>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
@@ -5777,14 +4641,14 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
       <c r="AE6" s="3">
-        <v>1</v>
+        <v>14.611000000000001</v>
       </c>
       <c r="AF6" s="3"/>
       <c r="AG6" s="3">
-        <v>1</v>
+        <v>14.611000000000001</v>
       </c>
       <c r="AH6" s="3">
-        <v>1</v>
+        <v>14.611000000000001</v>
       </c>
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
@@ -5798,7 +4662,7 @@
       <c r="AR6" s="3"/>
       <c r="AS6" s="3"/>
       <c r="AT6" s="3">
-        <v>3</v>
+        <v>24.491</v>
       </c>
     </row>
     <row r="7" spans="1:46">
@@ -5806,10 +4670,10 @@
         <v>2005</v>
       </c>
       <c r="B7" s="3">
-        <v>1</v>
+        <v>11.15</v>
       </c>
       <c r="C7" s="3">
-        <v>1</v>
+        <v>11.15</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -5820,7 +4684,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3">
-        <v>1</v>
+        <v>11.15</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -5851,18 +4715,18 @@
       <c r="AM7" s="3"/>
       <c r="AN7" s="3"/>
       <c r="AO7" s="3">
-        <v>1</v>
+        <v>6.7770000000000001</v>
       </c>
       <c r="AP7" s="3">
-        <v>1</v>
+        <v>6.7770000000000001</v>
       </c>
       <c r="AQ7" s="3"/>
       <c r="AR7" s="3"/>
       <c r="AS7" s="3">
-        <v>1</v>
+        <v>6.7770000000000001</v>
       </c>
       <c r="AT7" s="3">
-        <v>2</v>
+        <v>17.927</v>
       </c>
     </row>
     <row r="8" spans="1:46">
@@ -5872,10 +4736,10 @@
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3">
-        <v>1</v>
+        <v>0.126</v>
       </c>
       <c r="E8" s="3">
-        <v>1</v>
+        <v>0.126</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -5884,7 +4748,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3">
-        <v>1</v>
+        <v>0.126</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -5895,21 +4759,21 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3">
-        <v>1</v>
+        <v>11.807</v>
       </c>
       <c r="V8" s="3">
-        <v>1</v>
+        <v>11.807</v>
       </c>
       <c r="W8" s="3">
-        <v>1</v>
+        <v>11.807</v>
       </c>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="AA8" s="3">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
@@ -5918,7 +4782,7 @@
       <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
@@ -5929,16 +4793,16 @@
       <c r="AO8" s="3"/>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3">
-        <v>1</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="AR8" s="3">
-        <v>1</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="AS8" s="3">
-        <v>1</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="AT8" s="3">
-        <v>4</v>
+        <v>24.189999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:46">
@@ -5951,16 +4815,16 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3">
-        <v>1</v>
+        <v>2.78</v>
       </c>
       <c r="H9" s="3">
-        <v>1</v>
+        <v>2.78</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3">
-        <v>1</v>
+        <v>2.78</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -5996,7 +4860,7 @@
       <c r="AR9" s="3"/>
       <c r="AS9" s="3"/>
       <c r="AT9" s="3">
-        <v>1</v>
+        <v>2.78</v>
       </c>
     </row>
     <row r="10" spans="1:46">
@@ -6012,30 +4876,30 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3">
-        <v>1</v>
+        <v>3.077</v>
       </c>
       <c r="K10" s="3">
-        <v>1</v>
+        <v>3.077</v>
       </c>
       <c r="L10" s="3">
-        <v>1</v>
+        <v>3.077</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="R10" s="3">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
@@ -6046,13 +4910,13 @@
       <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3">
-        <v>1</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AG10" s="3">
-        <v>1</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AH10" s="3">
-        <v>1</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
@@ -6066,7 +4930,7 @@
       <c r="AR10" s="3"/>
       <c r="AS10" s="3"/>
       <c r="AT10" s="3">
-        <v>3</v>
+        <v>3.1829999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:46">
@@ -6074,119 +4938,119 @@
         <v>12</v>
       </c>
       <c r="B11" s="3">
-        <v>1</v>
+        <v>11.15</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
+        <v>11.15</v>
       </c>
       <c r="D11" s="3">
-        <v>1</v>
+        <v>0.126</v>
       </c>
       <c r="E11" s="3">
-        <v>1</v>
+        <v>0.126</v>
       </c>
       <c r="F11" s="3">
-        <v>1</v>
+        <v>3.99</v>
       </c>
       <c r="G11" s="3">
-        <v>1</v>
+        <v>2.78</v>
       </c>
       <c r="H11" s="3">
-        <v>2</v>
+        <v>6.77</v>
       </c>
       <c r="I11" s="3">
-        <v>1</v>
+        <v>7.27</v>
       </c>
       <c r="J11" s="3">
-        <v>1</v>
+        <v>3.077</v>
       </c>
       <c r="K11" s="3">
-        <v>2</v>
+        <v>10.347</v>
       </c>
       <c r="L11" s="3">
-        <v>6</v>
+        <v>28.393000000000001</v>
       </c>
       <c r="M11" s="3">
-        <v>1</v>
+        <v>5.77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="3">
-        <v>1</v>
+        <v>5.77</v>
       </c>
       <c r="P11" s="3">
-        <v>1</v>
+        <v>2.61</v>
       </c>
       <c r="Q11" s="3">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="R11" s="3">
-        <v>2</v>
+        <v>2.63</v>
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3">
-        <v>1</v>
+        <v>11.807</v>
       </c>
       <c r="V11" s="3">
-        <v>1</v>
+        <v>11.807</v>
       </c>
       <c r="W11" s="3">
-        <v>4</v>
+        <v>20.206999999999997</v>
       </c>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="AA11" s="3">
-        <v>1</v>
+        <v>3.69</v>
       </c>
       <c r="AB11" s="3">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3">
-        <v>1</v>
+        <v>4.3</v>
       </c>
       <c r="AE11" s="3">
-        <v>1</v>
+        <v>14.611000000000001</v>
       </c>
       <c r="AF11" s="3">
-        <v>1</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AG11" s="3">
-        <v>2</v>
+        <v>14.697000000000001</v>
       </c>
       <c r="AH11" s="3">
-        <v>4</v>
+        <v>22.687000000000001</v>
       </c>
       <c r="AI11" s="3">
-        <v>1</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3">
-        <v>1</v>
+        <v>10.039999999999999</v>
       </c>
       <c r="AL11" s="3"/>
       <c r="AM11" s="3"/>
       <c r="AN11" s="3"/>
       <c r="AO11" s="3">
-        <v>1</v>
+        <v>6.7770000000000001</v>
       </c>
       <c r="AP11" s="3">
-        <v>1</v>
+        <v>6.7770000000000001</v>
       </c>
       <c r="AQ11" s="3">
-        <v>1</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="AR11" s="3">
-        <v>1</v>
+        <v>8.5670000000000002</v>
       </c>
       <c r="AS11" s="3">
-        <v>3</v>
+        <v>25.384</v>
       </c>
       <c r="AT11" s="3">
-        <v>17</v>
+        <v>96.670999999999992</v>
       </c>
     </row>
   </sheetData>
@@ -6299,10 +5163,10 @@
         <v>10.039999999999999</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2">
-        <v>100001</v>
+        <v>77</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
       </c>
       <c r="G2" t="s">
         <v>38</v>
@@ -6331,10 +5195,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3">
-        <v>100002</v>
+        <v>78</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -6360,10 +5224,10 @@
         <v>6.7770000000000001</v>
       </c>
       <c r="D4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4">
-        <v>100003</v>
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
       </c>
       <c r="G4" t="s">
         <v>43</v>
@@ -6389,10 +5253,10 @@
         <v>8.5670000000000002</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5">
-        <v>100004</v>
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>88</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
@@ -6451,10 +5315,10 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6">
-        <v>100005</v>
+        <v>77</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
       </c>
       <c r="G6" t="s">
         <v>47</v>
@@ -6477,10 +5341,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7">
-        <v>100006</v>
+        <v>78</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
       </c>
       <c r="G7" t="s">
         <v>49</v>
@@ -6506,10 +5370,10 @@
         <v>3.99</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8">
-        <v>100007</v>
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
       </c>
       <c r="G8" t="s">
         <v>49</v>
@@ -6535,10 +5399,10 @@
         <v>7.27</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9">
-        <v>100008</v>
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>92</v>
       </c>
       <c r="G9" t="s">
         <v>49</v>
@@ -6570,10 +5434,10 @@
         <v>11.15</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10">
-        <v>100009</v>
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>93</v>
       </c>
       <c r="G10" t="s">
         <v>38</v>
@@ -6611,10 +5475,10 @@
         <v>0.126</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11">
-        <v>100010</v>
+        <v>78</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
       </c>
       <c r="G11" t="s">
         <v>38</v>
@@ -6646,10 +5510,10 @@
         <v>2.78</v>
       </c>
       <c r="D12" t="s">
-        <v>80</v>
-      </c>
-      <c r="E12">
-        <v>100011</v>
+        <v>79</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -6663,10 +5527,10 @@
         <v>3.077</v>
       </c>
       <c r="D13" t="s">
-        <v>81</v>
-      </c>
-      <c r="E13">
-        <v>100012</v>
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -6680,10 +5544,10 @@
         <v>5.77</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14">
-        <v>100013</v>
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -6697,10 +5561,10 @@
         <v>2.61</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15">
-        <v>100014</v>
+        <v>78</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -6711,10 +5575,10 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16">
-        <v>100015</v>
+        <v>79</v>
+      </c>
+      <c r="E16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -6728,10 +5592,10 @@
         <v>11.807</v>
       </c>
       <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17">
-        <v>100016</v>
+        <v>80</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -6742,10 +5606,10 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18">
-        <v>100017</v>
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -6759,10 +5623,10 @@
         <v>0.02</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19">
-        <v>100018</v>
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -6776,10 +5640,10 @@
         <v>4.3</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20">
-        <v>100019</v>
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -6793,10 +5657,10 @@
         <v>14.611000000000001</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21">
-        <v>100020</v>
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -6807,10 +5671,10 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22">
-        <v>100021</v>
+        <v>77</v>
+      </c>
+      <c r="E22" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -6824,10 +5688,10 @@
         <v>3.69</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23">
-        <v>100022</v>
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -6838,10 +5702,10 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24">
-        <v>100023</v>
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -6855,10 +5719,10 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25">
-        <v>100024</v>
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -7440,25 +6304,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:N20"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="A12:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="24" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" customWidth="1"/>
     <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14">
+    <row r="1" spans="1:14">
       <c r="C1" t="s">
         <v>59</v>
       </c>
@@ -7493,31 +6357,37 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:14">
+    <row r="2" spans="1:14">
       <c r="B2" s="3">
         <v>1993</v>
       </c>
       <c r="C2" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
         <v>1</v>
       </c>
       <c r="D2" s="5">
-        <v>2</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>6</v>
       </c>
       <c r="E2" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>7</v>
+      </c>
+      <c r="F2" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
+      </c>
+      <c r="G2" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
         <v>3</v>
       </c>
-      <c r="F2" s="5">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5">
-        <v>5</v>
-      </c>
-      <c r="H2" s="5">
-        <v>6</v>
-      </c>
       <c r="I2" t="str">
-        <f t="shared" ref="I2:I9" si="0">INDEX($C$1:$H$1, MATCH(MAX(C2:H2),C2:H2, 0))</f>
-        <v>Product 6</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C2:H2),C2:H2, 0))</f>
+        <v>Product 4</v>
       </c>
       <c r="K2">
         <v>1993</v>
@@ -7532,31 +6402,37 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:14">
+    <row r="3" spans="1:14">
       <c r="B3" s="3">
         <v>1994</v>
       </c>
       <c r="C3" s="5">
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>1</v>
       </c>
       <c r="D3" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>2</v>
       </c>
       <c r="E3" s="5">
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
       </c>
       <c r="F3" s="5">
-        <v>14</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="G3" s="5">
-        <v>15</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>3</v>
       </c>
       <c r="H3" s="5">
-        <v>16</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>1</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 6</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C3:H3),C3:H3, 0))</f>
+        <v>Product 4</v>
       </c>
       <c r="K3">
         <v>2001</v>
@@ -7568,31 +6444,37 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:14">
+    <row r="4" spans="1:14">
       <c r="B4" s="3">
         <v>1995</v>
       </c>
       <c r="C4" s="5">
-        <v>16</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>4</v>
       </c>
       <c r="D4" s="5">
-        <v>15</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>6</v>
       </c>
       <c r="E4" s="5">
-        <v>14</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>2</v>
       </c>
       <c r="F4" s="5">
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="G4" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>6</v>
       </c>
       <c r="H4" s="5">
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>7</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 1</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C4:H4),C4:H4, 0))</f>
+        <v>Product 4</v>
       </c>
       <c r="K4">
         <v>2005</v>
@@ -7607,31 +6489,37 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="1:14">
       <c r="B5" s="3">
         <v>1996</v>
       </c>
       <c r="C5" s="5">
-        <v>2</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>10</v>
       </c>
       <c r="D5" s="5">
-        <v>7</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>10</v>
       </c>
       <c r="E5" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="F5" s="5">
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>3</v>
       </c>
       <c r="G5" s="5">
-        <v>22</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>8</v>
       </c>
       <c r="H5" s="5">
-        <v>27</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 6</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C5:H5),C5:H5, 0))</f>
+        <v>Product 1</v>
       </c>
       <c r="K5">
         <v>2008</v>
@@ -7646,31 +6534,37 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="1:14">
       <c r="B6" s="3">
         <v>1997</v>
       </c>
       <c r="C6" s="5">
-        <v>25</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>8</v>
       </c>
       <c r="D6" s="5">
-        <v>22</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>3</v>
       </c>
       <c r="E6" s="5">
-        <v>19</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
       </c>
       <c r="F6" s="5">
-        <v>16</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>8</v>
       </c>
       <c r="G6" s="5">
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>1</v>
       </c>
       <c r="H6" s="5">
-        <v>10</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 1</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C6:H6),C6:H6, 0))</f>
+        <v>Product 6</v>
       </c>
       <c r="K6">
         <v>2010</v>
@@ -7682,31 +6576,37 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="2:14">
+    <row r="7" spans="1:14">
       <c r="B7" s="3">
         <v>1998</v>
       </c>
       <c r="C7" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
         <v>8</v>
       </c>
       <c r="D7" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
+      </c>
+      <c r="E7" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
         <v>2</v>
       </c>
-      <c r="E7" s="5">
-        <v>7</v>
-      </c>
       <c r="F7" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>6</v>
       </c>
       <c r="G7" s="5">
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>9</v>
       </c>
       <c r="H7" s="5">
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 5</v>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C7:H7),C7:H7, 0))</f>
+        <v>Product 2</v>
       </c>
       <c r="K7">
         <v>2011</v>
@@ -7718,311 +6618,147 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="1:14">
       <c r="B8" s="3">
         <v>1999</v>
       </c>
       <c r="C8" s="5">
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
       </c>
       <c r="D8" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>7</v>
+      </c>
+      <c r="E8" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>2</v>
+      </c>
+      <c r="F8" s="5">
+        <f ca="1">RANDBETWEEN(1, 10)</f>
         <v>5</v>
       </c>
-      <c r="E8" s="5">
-        <v>15</v>
-      </c>
-      <c r="F8" s="5">
-        <v>12</v>
-      </c>
       <c r="G8" s="5">
-        <v>22</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>3</v>
       </c>
       <c r="H8" s="5">
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>8</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C8:H8),C8:H8, 0))</f>
+        <v>Product 6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="3">
         <v>2000</v>
       </c>
       <c r="C9" s="5">
-        <v>14</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>5</v>
       </c>
       <c r="D9" s="5">
-        <v>11</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>2</v>
       </c>
       <c r="E9" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>4</v>
       </c>
       <c r="F9" s="5">
-        <v>13</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>2</v>
       </c>
       <c r="G9" s="5">
-        <v>14</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>3</v>
       </c>
       <c r="H9" s="5">
-        <v>12</v>
+        <f ca="1">RANDBETWEEN(1, 10)</f>
+        <v>7</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>Product 1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="C13" s="3">
-        <v>1993</v>
-      </c>
-      <c r="D13" s="5" t="str">
-        <f>C2&amp;", " &amp;D$12&amp;", " &amp; $C13</f>
-        <v>1, L1, 1993</v>
-      </c>
-      <c r="E13" s="5" t="str">
-        <f>D2&amp;", " &amp;E$12&amp;", " &amp; $C13</f>
-        <v>2, L2, 1993</v>
-      </c>
-      <c r="F13" s="5" t="str">
-        <f>E2&amp;", " &amp;F$12&amp;", " &amp; $C13</f>
-        <v>3, L3, 1993</v>
-      </c>
-      <c r="G13" s="5" t="str">
-        <f>F2&amp;", " &amp;G$12&amp;", " &amp; $C13</f>
-        <v>4, L4, 1993</v>
-      </c>
-      <c r="H13" s="5" t="str">
-        <f>G2&amp;", " &amp;H$12&amp;", " &amp; $C13</f>
-        <v>5, L5, 1993</v>
-      </c>
-      <c r="I13" s="5" t="str">
-        <f>H2&amp;", " &amp;I$12&amp;", " &amp; $C13</f>
-        <v>6, L6, 1993</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14">
-      <c r="C14" s="3">
-        <v>1994</v>
-      </c>
-      <c r="D14" s="5" t="str">
-        <f>C3&amp;", " &amp;D$12&amp;", " &amp; $C14</f>
-        <v>11, L1, 1994</v>
-      </c>
-      <c r="E14" s="5" t="str">
-        <f>D3&amp;", " &amp;E$12&amp;", " &amp; $C14</f>
-        <v>12, L2, 1994</v>
-      </c>
-      <c r="F14" s="5" t="str">
-        <f>E3&amp;", " &amp;F$12&amp;", " &amp; $C14</f>
-        <v>13, L3, 1994</v>
-      </c>
-      <c r="G14" s="5" t="str">
-        <f>F3&amp;", " &amp;G$12&amp;", " &amp; $C14</f>
-        <v>14, L4, 1994</v>
-      </c>
-      <c r="H14" s="5" t="str">
-        <f>G3&amp;", " &amp;H$12&amp;", " &amp; $C14</f>
-        <v>15, L5, 1994</v>
-      </c>
-      <c r="I14" s="5" t="str">
-        <f>H3&amp;", " &amp;I$12&amp;", " &amp; $C14</f>
-        <v>16, L6, 1994</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
-      <c r="C15" s="3">
-        <v>1995</v>
-      </c>
-      <c r="D15" s="5" t="str">
-        <f>C4&amp;", " &amp;D$12&amp;", " &amp; $C15</f>
-        <v>16, L1, 1995</v>
-      </c>
-      <c r="E15" s="5" t="str">
-        <f>D4&amp;", " &amp;E$12&amp;", " &amp; $C15</f>
-        <v>15, L2, 1995</v>
-      </c>
-      <c r="F15" s="5" t="str">
-        <f>E4&amp;", " &amp;F$12&amp;", " &amp; $C15</f>
-        <v>14, L3, 1995</v>
-      </c>
-      <c r="G15" s="5" t="str">
-        <f>F4&amp;", " &amp;G$12&amp;", " &amp; $C15</f>
-        <v>13, L4, 1995</v>
-      </c>
-      <c r="H15" s="5" t="str">
-        <f>G4&amp;", " &amp;H$12&amp;", " &amp; $C15</f>
-        <v>12, L5, 1995</v>
-      </c>
-      <c r="I15" s="5" t="str">
-        <f>H4&amp;", " &amp;I$12&amp;", " &amp; $C15</f>
-        <v>11, L6, 1995</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="C16" s="3">
-        <v>1996</v>
-      </c>
-      <c r="D16" s="5" t="str">
-        <f>C5&amp;", " &amp;D$12&amp;", " &amp; $C16</f>
-        <v>2, L1, 1996</v>
-      </c>
-      <c r="E16" s="5" t="str">
-        <f>D5&amp;", " &amp;E$12&amp;", " &amp; $C16</f>
-        <v>7, L2, 1996</v>
-      </c>
-      <c r="F16" s="5" t="str">
-        <f>E5&amp;", " &amp;F$12&amp;", " &amp; $C16</f>
-        <v>12, L3, 1996</v>
-      </c>
-      <c r="G16" s="5" t="str">
-        <f>F5&amp;", " &amp;G$12&amp;", " &amp; $C16</f>
-        <v>17, L4, 1996</v>
-      </c>
-      <c r="H16" s="5" t="str">
-        <f>G5&amp;", " &amp;H$12&amp;", " &amp; $C16</f>
-        <v>22, L5, 1996</v>
-      </c>
-      <c r="I16" s="5" t="str">
-        <f>H5&amp;", " &amp;I$12&amp;", " &amp; $C16</f>
-        <v>27, L6, 1996</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9">
-      <c r="C17" s="3">
-        <v>1997</v>
-      </c>
-      <c r="D17" s="5" t="str">
-        <f>C6&amp;", " &amp;D$12&amp;", " &amp; $C17</f>
-        <v>25, L1, 1997</v>
-      </c>
-      <c r="E17" s="5" t="str">
-        <f>D6&amp;", " &amp;E$12&amp;", " &amp; $C17</f>
-        <v>22, L2, 1997</v>
-      </c>
-      <c r="F17" s="5" t="str">
-        <f>E6&amp;", " &amp;F$12&amp;", " &amp; $C17</f>
-        <v>19, L3, 1997</v>
-      </c>
-      <c r="G17" s="5" t="str">
-        <f>F6&amp;", " &amp;G$12&amp;", " &amp; $C17</f>
-        <v>16, L4, 1997</v>
-      </c>
-      <c r="H17" s="5" t="str">
-        <f>G6&amp;", " &amp;H$12&amp;", " &amp; $C17</f>
-        <v>13, L5, 1997</v>
-      </c>
-      <c r="I17" s="5" t="str">
-        <f>H6&amp;", " &amp;I$12&amp;", " &amp; $C17</f>
-        <v>10, L6, 1997</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9">
-      <c r="C18" s="3">
-        <v>1998</v>
-      </c>
-      <c r="D18" s="5" t="str">
-        <f>C7&amp;", " &amp;D$12&amp;", " &amp; $C18</f>
-        <v>8, L1, 1998</v>
-      </c>
-      <c r="E18" s="5" t="str">
-        <f>D7&amp;", " &amp;E$12&amp;", " &amp; $C18</f>
-        <v>2, L2, 1998</v>
-      </c>
-      <c r="F18" s="5" t="str">
-        <f>E7&amp;", " &amp;F$12&amp;", " &amp; $C18</f>
-        <v>7, L3, 1998</v>
-      </c>
-      <c r="G18" s="5" t="str">
-        <f>F7&amp;", " &amp;G$12&amp;", " &amp; $C18</f>
-        <v>12, L4, 1998</v>
-      </c>
-      <c r="H18" s="5" t="str">
-        <f>G7&amp;", " &amp;H$12&amp;", " &amp; $C18</f>
-        <v>17, L5, 1998</v>
-      </c>
-      <c r="I18" s="5" t="str">
-        <f>H7&amp;", " &amp;I$12&amp;", " &amp; $C18</f>
-        <v>11, L6, 1998</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9">
-      <c r="C19" s="3">
-        <v>1999</v>
-      </c>
-      <c r="D19" s="5" t="str">
-        <f>C8&amp;", " &amp;D$12&amp;", " &amp; $C19</f>
-        <v>11, L1, 1999</v>
-      </c>
-      <c r="E19" s="5" t="str">
-        <f>D8&amp;", " &amp;E$12&amp;", " &amp; $C19</f>
-        <v>5, L2, 1999</v>
-      </c>
-      <c r="F19" s="5" t="str">
-        <f>E8&amp;", " &amp;F$12&amp;", " &amp; $C19</f>
-        <v>15, L3, 1999</v>
-      </c>
-      <c r="G19" s="5" t="str">
-        <f>F8&amp;", " &amp;G$12&amp;", " &amp; $C19</f>
-        <v>12, L4, 1999</v>
-      </c>
-      <c r="H19" s="5" t="str">
-        <f>G8&amp;", " &amp;H$12&amp;", " &amp; $C19</f>
-        <v>22, L5, 1999</v>
-      </c>
-      <c r="I19" s="5" t="str">
-        <f>H8&amp;", " &amp;I$12&amp;", " &amp; $C19</f>
-        <v>13, L6, 1999</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9">
-      <c r="C20" s="3">
-        <v>2000</v>
-      </c>
-      <c r="D20" s="5" t="str">
-        <f>C9&amp;", " &amp;D$12&amp;", " &amp; $C20</f>
-        <v>14, L1, 2000</v>
-      </c>
-      <c r="E20" s="5" t="str">
-        <f>D9&amp;", " &amp;E$12&amp;", " &amp; $C20</f>
-        <v>11, L2, 2000</v>
-      </c>
-      <c r="F20" s="5" t="str">
-        <f>E9&amp;", " &amp;F$12&amp;", " &amp; $C20</f>
-        <v>12, L3, 2000</v>
-      </c>
-      <c r="G20" s="5" t="str">
-        <f>F9&amp;", " &amp;G$12&amp;", " &amp; $C20</f>
-        <v>13, L4, 2000</v>
-      </c>
-      <c r="H20" s="5" t="str">
-        <f>G9&amp;", " &amp;H$12&amp;", " &amp; $C20</f>
-        <v>14, L5, 2000</v>
-      </c>
-      <c r="I20" s="5" t="str">
-        <f>H9&amp;", " &amp;I$12&amp;", " &amp; $C20</f>
-        <v>12, L6, 2000</v>
-      </c>
+        <f ca="1">INDEX($C$1:$H$1, MATCH(MAX(C9:H9),C9:H9, 0))</f>
+        <v>Product 6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="3"/>
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="3"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="3"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="3"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="3"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="3"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8438,4 +7174,302 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="3"/>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1993</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;C$1&amp;", " &amp;formula!C2&amp;", " &amp; $A2</f>
+        <v>1993, L1, 1, Treatment 01</v>
+      </c>
+      <c r="D2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;D$1&amp;", " &amp;formula!D2&amp;", " &amp; $A2</f>
+        <v>1993, L2, 6, Treatment 01</v>
+      </c>
+      <c r="E2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;E$1&amp;", " &amp;formula!E2&amp;", " &amp; $A2</f>
+        <v>1993, L3, 7, Treatment 01</v>
+      </c>
+      <c r="F2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;F$1&amp;", " &amp;formula!F2&amp;", " &amp; $A2</f>
+        <v>1993, L4, 9, Treatment 01</v>
+      </c>
+      <c r="G2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;G$1&amp;", " &amp;formula!G2&amp;", " &amp; $A2</f>
+        <v>1993, L5, 5, Treatment 01</v>
+      </c>
+      <c r="H2" s="5" t="str">
+        <f ca="1">$B2&amp;", "&amp;H$1&amp;", " &amp;formula!H2&amp;", " &amp; $A2</f>
+        <v>1993, L6, 3, Treatment 01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1994</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;C$1&amp;", " &amp;formula!C3&amp;", " &amp; $A3</f>
+        <v>1994, L1, 1, Treatment 02</v>
+      </c>
+      <c r="D3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;D$1&amp;", " &amp;formula!D3&amp;", " &amp; $A3</f>
+        <v>1994, L2, 2, Treatment 02</v>
+      </c>
+      <c r="E3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;E$1&amp;", " &amp;formula!E3&amp;", " &amp; $A3</f>
+        <v>1994, L3, 5, Treatment 02</v>
+      </c>
+      <c r="F3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;F$1&amp;", " &amp;formula!F3&amp;", " &amp; $A3</f>
+        <v>1994, L4, 9, Treatment 02</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;G$1&amp;", " &amp;formula!G3&amp;", " &amp; $A3</f>
+        <v>1994, L5, 3, Treatment 02</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f ca="1">$B3&amp;", "&amp;H$1&amp;", " &amp;formula!H3&amp;", " &amp; $A3</f>
+        <v>1994, L6, 1, Treatment 02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1995</v>
+      </c>
+      <c r="C4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;C$1&amp;", " &amp;formula!C4&amp;", " &amp; $A4</f>
+        <v>1995, L1, 4, Treatment 03</v>
+      </c>
+      <c r="D4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;D$1&amp;", " &amp;formula!D4&amp;", " &amp; $A4</f>
+        <v>1995, L2, 6, Treatment 03</v>
+      </c>
+      <c r="E4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;E$1&amp;", " &amp;formula!E4&amp;", " &amp; $A4</f>
+        <v>1995, L3, 2, Treatment 03</v>
+      </c>
+      <c r="F4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;F$1&amp;", " &amp;formula!F4&amp;", " &amp; $A4</f>
+        <v>1995, L4, 9, Treatment 03</v>
+      </c>
+      <c r="G4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;G$1&amp;", " &amp;formula!G4&amp;", " &amp; $A4</f>
+        <v>1995, L5, 6, Treatment 03</v>
+      </c>
+      <c r="H4" s="5" t="str">
+        <f ca="1">$B4&amp;", "&amp;H$1&amp;", " &amp;formula!H4&amp;", " &amp; $A4</f>
+        <v>1995, L6, 7, Treatment 03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1996</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;C$1&amp;", " &amp;formula!C5&amp;", " &amp; $A5</f>
+        <v>1996, L1, 10, Treatment 04</v>
+      </c>
+      <c r="D5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;D$1&amp;", " &amp;formula!D5&amp;", " &amp; $A5</f>
+        <v>1996, L2, 10, Treatment 04</v>
+      </c>
+      <c r="E5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;E$1&amp;", " &amp;formula!E5&amp;", " &amp; $A5</f>
+        <v>1996, L3, 9, Treatment 04</v>
+      </c>
+      <c r="F5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;F$1&amp;", " &amp;formula!F5&amp;", " &amp; $A5</f>
+        <v>1996, L4, 3, Treatment 04</v>
+      </c>
+      <c r="G5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;G$1&amp;", " &amp;formula!G5&amp;", " &amp; $A5</f>
+        <v>1996, L5, 8, Treatment 04</v>
+      </c>
+      <c r="H5" s="5" t="str">
+        <f ca="1">$B5&amp;", "&amp;H$1&amp;", " &amp;formula!H5&amp;", " &amp; $A5</f>
+        <v>1996, L6, 9, Treatment 04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1997</v>
+      </c>
+      <c r="C6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;C$1&amp;", " &amp;formula!C6&amp;", " &amp; $A6</f>
+        <v>1997, L1, 8, Treatment 05</v>
+      </c>
+      <c r="D6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;D$1&amp;", " &amp;formula!D6&amp;", " &amp; $A6</f>
+        <v>1997, L2, 3, Treatment 05</v>
+      </c>
+      <c r="E6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;E$1&amp;", " &amp;formula!E6&amp;", " &amp; $A6</f>
+        <v>1997, L3, 5, Treatment 05</v>
+      </c>
+      <c r="F6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;F$1&amp;", " &amp;formula!F6&amp;", " &amp; $A6</f>
+        <v>1997, L4, 8, Treatment 05</v>
+      </c>
+      <c r="G6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;G$1&amp;", " &amp;formula!G6&amp;", " &amp; $A6</f>
+        <v>1997, L5, 1, Treatment 05</v>
+      </c>
+      <c r="H6" s="5" t="str">
+        <f ca="1">$B6&amp;", "&amp;H$1&amp;", " &amp;formula!H6&amp;", " &amp; $A6</f>
+        <v>1997, L6, 9, Treatment 05</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1998</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;C$1&amp;", " &amp;formula!C7&amp;", " &amp; $A7</f>
+        <v>1998, L1, 8, Treatment 06</v>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;D$1&amp;", " &amp;formula!D7&amp;", " &amp; $A7</f>
+        <v>1998, L2, 9, Treatment 06</v>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;E$1&amp;", " &amp;formula!E7&amp;", " &amp; $A7</f>
+        <v>1998, L3, 2, Treatment 06</v>
+      </c>
+      <c r="F7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;F$1&amp;", " &amp;formula!F7&amp;", " &amp; $A7</f>
+        <v>1998, L4, 6, Treatment 06</v>
+      </c>
+      <c r="G7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;G$1&amp;", " &amp;formula!G7&amp;", " &amp; $A7</f>
+        <v>1998, L5, 9, Treatment 06</v>
+      </c>
+      <c r="H7" s="5" t="str">
+        <f ca="1">$B7&amp;", "&amp;H$1&amp;", " &amp;formula!H7&amp;", " &amp; $A7</f>
+        <v>1998, L6, 5, Treatment 06</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1999</v>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;C$1&amp;", " &amp;formula!C8&amp;", " &amp; $A8</f>
+        <v>1999, L1, 5, Treatment 07</v>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;D$1&amp;", " &amp;formula!D8&amp;", " &amp; $A8</f>
+        <v>1999, L2, 7, Treatment 07</v>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;E$1&amp;", " &amp;formula!E8&amp;", " &amp; $A8</f>
+        <v>1999, L3, 2, Treatment 07</v>
+      </c>
+      <c r="F8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;F$1&amp;", " &amp;formula!F8&amp;", " &amp; $A8</f>
+        <v>1999, L4, 5, Treatment 07</v>
+      </c>
+      <c r="G8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;G$1&amp;", " &amp;formula!G8&amp;", " &amp; $A8</f>
+        <v>1999, L5, 3, Treatment 07</v>
+      </c>
+      <c r="H8" s="5" t="str">
+        <f ca="1">$B8&amp;", "&amp;H$1&amp;", " &amp;formula!H8&amp;", " &amp; $A8</f>
+        <v>1999, L6, 8, Treatment 07</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;C$1&amp;", " &amp;formula!C9&amp;", " &amp; $A9</f>
+        <v>2000, L1, 5, Treatment 08</v>
+      </c>
+      <c r="D9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;D$1&amp;", " &amp;formula!D9&amp;", " &amp; $A9</f>
+        <v>2000, L2, 2, Treatment 08</v>
+      </c>
+      <c r="E9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;E$1&amp;", " &amp;formula!E9&amp;", " &amp; $A9</f>
+        <v>2000, L3, 4, Treatment 08</v>
+      </c>
+      <c r="F9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;F$1&amp;", " &amp;formula!F9&amp;", " &amp; $A9</f>
+        <v>2000, L4, 2, Treatment 08</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;G$1&amp;", " &amp;formula!G9&amp;", " &amp; $A9</f>
+        <v>2000, L5, 3, Treatment 08</v>
+      </c>
+      <c r="H9" s="5" t="str">
+        <f ca="1">$B9&amp;", "&amp;H$1&amp;", " &amp;formula!H9&amp;", " &amp; $A9</f>
+        <v>2000, L6, 7, Treatment 08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>